<commit_message>
add flan redu gasket
</commit_message>
<xml_diff>
--- a/resourse/reflaction.xlsx
+++ b/resourse/reflaction.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codes\PML _auto\resourse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5368E3-79BB-4761-A212-BE09C932EA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD27BD49-F902-4806-9F0D-1E867DD67E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="1140" windowWidth="22980" windowHeight="12195" activeTab="3" xr2:uid="{C5EB657E-11B3-40E4-A5D9-D81D34CEC6F4}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="16200" windowHeight="11100" activeTab="4" xr2:uid="{C5EB657E-11B3-40E4-A5D9-D81D34CEC6F4}"/>
   </bookViews>
   <sheets>
     <sheet name="elbow" sheetId="1" r:id="rId1"/>
     <sheet name="tube" sheetId="2" r:id="rId2"/>
     <sheet name="tee" sheetId="3" r:id="rId3"/>
     <sheet name="redu" sheetId="4" r:id="rId4"/>
-    <sheet name="flan" sheetId="5" r:id="rId5"/>
+    <sheet name="gask" sheetId="6" r:id="rId5"/>
+    <sheet name="flan" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="535">
   <si>
     <t>/NJU-SPEC/ELBO-1</t>
   </si>
@@ -1580,6 +1581,69 @@
   </si>
   <si>
     <t>/NJU-SPEC/REDU-156</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-1</t>
+  </si>
+  <si>
+    <t>GASK</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-2</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-3</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-4</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-5</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-6</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-7</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-8</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-9</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-10</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-11</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-12</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-13</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-14</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-15</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-16</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-17</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-18</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-19</t>
+  </si>
+  <si>
+    <t>/NJU-SPEC/GASK-20</t>
   </si>
 </sst>
 </file>
@@ -9735,7 +9799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2103B1D7-5869-4875-99B2-89347FE2EFE4}">
   <dimension ref="A1:N156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -13492,6 +13556,442 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF41A6E-C43B-48E0-99D3-5924B41FA9FB}">
+  <dimension ref="A1:M20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C1" s="1">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C2" s="1">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C3" s="1">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C4" s="1">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C5" s="1">
+        <v>40</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C6" s="1">
+        <v>50</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C7" s="1">
+        <v>65</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C8" s="1">
+        <v>80</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C9" s="1">
+        <v>100</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C10" s="1">
+        <v>125</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C11" s="1">
+        <v>150</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C12" s="1">
+        <v>200</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C13" s="1">
+        <v>250</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C14" s="1">
+        <v>300</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C15" s="1">
+        <v>350</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C16" s="1">
+        <v>400</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C17" s="1">
+        <v>450</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C18" s="1">
+        <v>500</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C19" s="1">
+        <v>550</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C20" s="1">
+        <v>600</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2596A408-01AF-4336-B266-855C710E0BBC}">
   <dimension ref="A1:M28"/>
   <sheetViews>

</xml_diff>